<commit_message>
download file chi tiet giao dich
</commit_message>
<xml_diff>
--- a/framework/configuration.xlsx
+++ b/framework/configuration.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="173">
   <si>
     <t>key</t>
   </si>
@@ -508,13 +508,52 @@
   </si>
   <si>
     <t>0-bank account, 1-fdate, 2-tdate</t>
+  </si>
+  <si>
+    <t>VIETQR_FILE</t>
+  </si>
+  <si>
+    <t>BANK_SUMMARY_FILE</t>
+  </si>
+  <si>
+    <t>VIETQR_SUMMARY_FILE</t>
+  </si>
+  <si>
+    <t>{PROCESS_DATA}\bank_summary.xlsx</t>
+  </si>
+  <si>
+    <t>{PROCESS_DATA}\vietqr_summary.xlsx</t>
+  </si>
+  <si>
+    <t>REPORT_GSHEET</t>
+  </si>
+  <si>
+    <t>1CeajU4bSSNsok4PoY_uBCPEzl0Q81yrG4hRBMq-PulE</t>
+  </si>
+  <si>
+    <t>VIETQR_PASSWORD</t>
+  </si>
+  <si>
+    <t>VIETQR_USERNAME</t>
+  </si>
+  <si>
+    <t>0984295800</t>
+  </si>
+  <si>
+    <t>BANK_ACCOUNT</t>
+  </si>
+  <si>
+    <t>3991031291095</t>
+  </si>
+  <si>
+    <t>{PROCESS_DATA}\vietqr_{0}_{1}.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -581,6 +620,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Open Sans"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -609,7 +654,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -660,6 +705,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -860,8 +917,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E68" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A1:E68"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E70" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A1:E70"/>
   <tableColumns count="5">
     <tableColumn id="1" name="key" dataDxfId="4"/>
     <tableColumn id="5" name="env" dataDxfId="3"/>
@@ -1143,24 +1200,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="30.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.69921875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.796875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="30.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.75" style="3" customWidth="1"/>
     <col min="4" max="4" width="14" style="3" customWidth="1"/>
-    <col min="5" max="5" width="68.296875" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.796875" style="3"/>
+    <col min="5" max="5" width="68.25" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.75" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1275,7 +1332,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
@@ -1374,7 +1431,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.6">
+    <row r="16" spans="1:5" ht="15.75">
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
@@ -1389,7 +1446,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="15">
       <c r="A17" s="7" t="s">
         <v>16</v>
       </c>
@@ -1442,7 +1499,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" ht="15">
       <c r="A22" s="7" t="s">
         <v>149</v>
       </c>
@@ -1451,7 +1508,7 @@
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" ht="15">
       <c r="A23" s="3" t="s">
         <v>147</v>
       </c>
@@ -1460,15 +1517,15 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" ht="15">
       <c r="C24" s="10"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" ht="15">
       <c r="C25" s="10"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" ht="15">
       <c r="A26" s="7" t="s">
         <v>104</v>
       </c>
@@ -1499,13 +1556,19 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="16"/>
+      <c r="A29" s="16" t="s">
+        <v>160</v>
+      </c>
       <c r="B29" s="17"/>
-      <c r="C29" s="10"/>
+      <c r="C29" s="10" t="s">
+        <v>172</v>
+      </c>
       <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="E29" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15">
       <c r="A30" s="7" t="s">
         <v>132</v>
       </c>
@@ -1515,178 +1578,171 @@
       <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="C31" s="10"/>
+      <c r="A31" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="B31" s="18"/>
+      <c r="C31" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+    </row>
+    <row r="34" spans="1:5" ht="15">
+      <c r="A34" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
+      <c r="A36" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>122</v>
+        <v>55</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>128</v>
-      </c>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15">
+      <c r="A38" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="27.6">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C40" s="11">
-        <v>3</v>
+        <v>126</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E40" s="15" t="s">
-        <v>133</v>
+        <v>22</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>116</v>
+        <v>145</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="28.5">
       <c r="A42" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
+      </c>
+      <c r="C42" s="11">
+        <v>3</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>119</v>
+        <v>21</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B43" s="3">
-        <v>10</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>146</v>
+        <v>115</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B44" s="3">
-        <v>20</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1694,271 +1750,277 @@
         <v>137</v>
       </c>
       <c r="B45" s="3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E45" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46" s="3">
+        <v>20</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B47" s="3">
+        <v>30</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15">
+      <c r="A48" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" s="7"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+    </row>
+    <row r="49" spans="1:5" ht="15">
+      <c r="A49" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C49" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E47" s="3" t="s">
+      <c r="D49" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E50" s="4" t="s">
-        <v>91</v>
+      <c r="E50" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>93</v>
+        <v>29</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E52" s="3" t="s">
-        <v>94</v>
+      <c r="E52" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>107</v>
+        <v>30</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E53" s="3" t="s">
-        <v>79</v>
+      <c r="E53" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C54" s="11">
-        <v>587</v>
+        <v>58</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>142</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" s="11">
+        <v>587</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15">
+      <c r="A57" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15">
+      <c r="A58" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E56" s="3" t="s">
+      <c r="D58" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>73</v>
+        <v>34</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>78</v>
+        <v>33</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>22</v>
@@ -1969,46 +2031,98 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E65" s="3" t="s">
+      <c r="D67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A66" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A67" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1">
       <c r="A68" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A69" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A70" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E68" s="3" t="s">
+      <c r="D70" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E70" s="3" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C72" s="3">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C73" s="21" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C74" s="21" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>